<commit_message>
fixed group model test
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data_linear.xlsx
+++ b/tests/data/ci_v2_data_linear.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedpreist/CodingStuff/DIMPACT/eam-core-provenance/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB04E13-6371-6D41-8109-C2430B917F1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8089C8E5-0369-2246-B405-FFEE3DFD08B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20960" windowHeight="16240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>variable</t>
   </si>
@@ -222,14 +222,19 @@
   </si>
   <si>
     <t>data vol</t>
+  </si>
+  <si>
+    <t>cdn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="195" formatCode="0.00000000000000000000000000000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -384,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -410,6 +415,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,18 +800,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="26" max="26" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -868,7 +877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -909,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -950,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -982,7 +991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1020,7 +1029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1058,16 +1067,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
@@ -1083,7 +1092,7 @@
         <v>36000000</v>
       </c>
       <c r="M9" s="18">
-        <f t="shared" ref="L9:X9" si="0">$F2</f>
+        <f t="shared" ref="M9:X9" si="0">$F2</f>
         <v>36000000</v>
       </c>
       <c r="N9" s="18">
@@ -1131,7 +1140,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -1200,7 +1209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="11"/>
       <c r="E11" s="9" t="s">
@@ -1214,59 +1223,59 @@
         <v>30</v>
       </c>
       <c r="L11">
-        <f>$F4</f>
+        <f t="shared" ref="L11:X11" si="3">$F4</f>
         <v>20</v>
       </c>
       <c r="M11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="O11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="P11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="Q11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="R11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="S11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="T11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="U11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="V11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="W11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="X11" s="18">
-        <f>$F4</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
         <v>41</v>
       </c>
@@ -1286,55 +1295,55 @@
         <v>1000000</v>
       </c>
       <c r="M12" s="24">
-        <f t="shared" ref="L12:X12" si="3">$F5</f>
+        <f t="shared" ref="M12:X12" si="4">$F5</f>
         <v>1000000</v>
       </c>
       <c r="N12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="O12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="P12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="Q12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="R12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="S12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="T12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="U12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="V12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="W12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="X12" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>43</v>
       </c>
       <c r="F13" s="11">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>35</v>
@@ -1355,55 +1364,55 @@
         <v>0.5</v>
       </c>
       <c r="M13" s="18">
-        <f t="shared" ref="L13:X13" si="4">$F6</f>
+        <f t="shared" ref="M13:X13" si="5">$F6</f>
         <v>0.5</v>
       </c>
       <c r="N13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="O13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="P13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="Q13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="R13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="S13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="U13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="V13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="W13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="X13" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
@@ -1418,7 +1427,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="E15" s="12" t="s">
         <v>45</v>
       </c>
@@ -1432,60 +1441,64 @@
       <c r="K15" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="26">
         <f>L9*$F10*L10*$F11*$F13</f>
-        <v>2.6000000000000003E-3</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="M15" s="16">
-        <f>M9*$F10*M10*$F11*$F13</f>
-        <v>2.7300000000000002E-3</v>
+        <f t="shared" ref="L15:X15" si="6">M9*$F10*M10*$F11*$F13</f>
+        <v>2.1000000000000001E-4</v>
       </c>
       <c r="N15" s="16">
-        <f>N9*$F10*N10*$F11*$F13</f>
-        <v>2.8600000000000001E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="O15" s="16">
-        <f>O9*$F10*O10*$F11*$F13</f>
-        <v>2.99E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.3000000000000001E-4</v>
       </c>
       <c r="P15" s="16">
-        <f>P9*$F10*P10*$F11*$F13</f>
-        <v>3.1199999999999999E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="Q15" s="16">
-        <f>Q9*$F10*Q10*$F11*$F13</f>
-        <v>3.2500000000000003E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="R15" s="16">
-        <f>R9*$F10*R10*$F11*$F13</f>
-        <v>3.3800000000000002E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.6000000000000003E-4</v>
       </c>
       <c r="S15" s="16">
-        <f>S9*$F10*S10*$F11*$F13</f>
-        <v>3.5100000000000001E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.7E-4</v>
       </c>
       <c r="T15" s="16">
-        <f>T9*$F10*T10*$F11*$F13</f>
-        <v>3.6400000000000004E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.8000000000000003E-4</v>
       </c>
       <c r="U15" s="16">
-        <f>U9*$F10*U10*$F11*$F13</f>
-        <v>3.7699999999999999E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.9E-4</v>
       </c>
       <c r="V15" s="16">
-        <f>V9*$F10*V10*$F11*$F13</f>
-        <v>3.9000000000000003E-3</v>
+        <f t="shared" si="6"/>
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="W15" s="16">
-        <f>W9*$F10*W10*$F11*$F13</f>
-        <v>4.0299999999999997E-3</v>
+        <f t="shared" si="6"/>
+        <v>3.1E-4</v>
       </c>
       <c r="X15" s="16">
-        <f>X9*$F10*X10*$F11*$F13</f>
-        <v>4.1600000000000005E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="Z15" s="27">
+        <f>SUM(L15:X15)</f>
+        <v>3.3799999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="K16" s="23" t="s">
         <v>61</v>
       </c>
@@ -1494,55 +1507,55 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="M16" s="24">
-        <f t="shared" ref="M16:X16" si="5">M10*M12*$F12</f>
+        <f t="shared" ref="M16:X16" si="7">M10*M12*$F12</f>
         <v>2.6250000000000002E-3</v>
       </c>
       <c r="N16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.7500000000000003E-3</v>
       </c>
       <c r="O16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8750000000000004E-3</v>
       </c>
       <c r="P16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Q16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="R16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.2500000000000003E-3</v>
       </c>
       <c r="S16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.3750000000000004E-3</v>
       </c>
       <c r="T16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="U16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6250000000000002E-3</v>
       </c>
       <c r="V16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.7500000000000003E-3</v>
       </c>
       <c r="W16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.8750000000000004E-3</v>
       </c>
       <c r="X16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>46</v>
       </c>
@@ -1560,26 +1573,26 @@
       <c r="H17" s="14"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B18" s="9"/>
       <c r="D18" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="16">
         <f>C9*F10*C10*F11*F13</f>
-        <v>2.6000000000000003E-3</v>
-      </c>
-      <c r="F18" s="17">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F18" s="24">
         <f>C10*F5*F12</f>
         <v>1.25E-3</v>
       </c>
       <c r="G18">
         <f>E18*F6/1000</f>
-        <v>1.3000000000000003E-6</v>
+        <v>1.0000000000000001E-7</v>
       </c>
       <c r="I18" s="11">
         <f>(E18+E19)/2</f>
-        <v>2.0222222222222226E-3</v>
+        <v>1.5555555555555556E-4</v>
       </c>
       <c r="J18" s="23" t="s">
         <v>60</v>
@@ -1587,15 +1600,71 @@
       <c r="K18" s="23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="24">
+        <f>L16*L11*$F13*$F14</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="M18" s="24">
+        <f t="shared" ref="M18:X18" si="8">M16*M11*$F13*$F14</f>
+        <v>5.25E-8</v>
+      </c>
+      <c r="N18" s="24">
+        <f t="shared" si="8"/>
+        <v>5.5000000000000003E-8</v>
+      </c>
+      <c r="O18" s="24">
+        <f t="shared" si="8"/>
+        <v>5.7500000000000005E-8</v>
+      </c>
+      <c r="P18" s="24">
+        <f t="shared" si="8"/>
+        <v>5.9999999999999995E-8</v>
+      </c>
+      <c r="Q18" s="24">
+        <f t="shared" si="8"/>
+        <v>6.2499999999999997E-8</v>
+      </c>
+      <c r="R18" s="24">
+        <f t="shared" si="8"/>
+        <v>6.5E-8</v>
+      </c>
+      <c r="S18" s="24">
+        <f t="shared" si="8"/>
+        <v>6.7500000000000002E-8</v>
+      </c>
+      <c r="T18" s="24">
+        <f t="shared" si="8"/>
+        <v>7.0000000000000005E-8</v>
+      </c>
+      <c r="U18" s="24">
+        <f t="shared" si="8"/>
+        <v>7.2500000000000007E-8</v>
+      </c>
+      <c r="V18" s="24">
+        <f t="shared" si="8"/>
+        <v>7.500000000000001E-8</v>
+      </c>
+      <c r="W18" s="24">
+        <f t="shared" si="8"/>
+        <v>7.7500000000000012E-8</v>
+      </c>
+      <c r="X18" s="24">
+        <f t="shared" si="8"/>
+        <v>8.0000000000000002E-8</v>
+      </c>
+      <c r="Z18" s="27">
+        <f>SUM(L18:X18)</f>
+        <v>8.4500000000000006E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B19" s="9"/>
       <c r="D19" t="s">
         <v>41</v>
       </c>
       <c r="E19" s="16">
         <f>C13*C14*F10*F11*F13</f>
-        <v>1.4444444444444446E-3</v>
+        <v>1.1111111111111112E-4</v>
       </c>
       <c r="F19" s="17">
         <f>C14*F5*F12</f>
@@ -1603,18 +1672,73 @@
       </c>
       <c r="G19" s="18">
         <f>E19*F6/1000</f>
-        <v>7.2222222222222225E-7</v>
+        <v>5.5555555555555561E-8</v>
       </c>
       <c r="I19" s="11">
         <f>(G18+G19)/2</f>
-        <v>1.0111111111111114E-6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+        <v>7.7777777777777782E-8</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="24">
+        <f>L16</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="M19" s="24">
+        <f t="shared" ref="M19:X19" si="9">M16</f>
+        <v>2.6250000000000002E-3</v>
+      </c>
+      <c r="N19" s="24">
+        <f t="shared" si="9"/>
+        <v>2.7500000000000003E-3</v>
+      </c>
+      <c r="O19" s="24">
+        <f t="shared" si="9"/>
+        <v>2.8750000000000004E-3</v>
+      </c>
+      <c r="P19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="R19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.2500000000000003E-3</v>
+      </c>
+      <c r="S19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.3750000000000004E-3</v>
+      </c>
+      <c r="T19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="U19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.6250000000000002E-3</v>
+      </c>
+      <c r="V19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.7500000000000003E-3</v>
+      </c>
+      <c r="W19" s="24">
+        <f t="shared" si="9"/>
+        <v>3.8750000000000004E-3</v>
+      </c>
+      <c r="X19" s="24">
+        <f t="shared" si="9"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="9"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>50</v>
       </c>
@@ -1628,15 +1752,77 @@
         <v>49</v>
       </c>
       <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J21" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="24">
+        <f>L19*L11*$F14*$F13</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="M21" s="24">
+        <f t="shared" ref="M21:X21" si="10">M19*M11*$F14*$F13</f>
+        <v>5.25E-8</v>
+      </c>
+      <c r="N21" s="24">
+        <f t="shared" si="10"/>
+        <v>5.5000000000000003E-8</v>
+      </c>
+      <c r="O21" s="24">
+        <f t="shared" si="10"/>
+        <v>5.7500000000000005E-8</v>
+      </c>
+      <c r="P21" s="24">
+        <f t="shared" si="10"/>
+        <v>5.9999999999999995E-8</v>
+      </c>
+      <c r="Q21" s="24">
+        <f t="shared" si="10"/>
+        <v>6.2499999999999997E-8</v>
+      </c>
+      <c r="R21" s="24">
+        <f t="shared" si="10"/>
+        <v>6.5E-8</v>
+      </c>
+      <c r="S21" s="24">
+        <f t="shared" si="10"/>
+        <v>6.7500000000000002E-8</v>
+      </c>
+      <c r="T21" s="24">
+        <f t="shared" si="10"/>
+        <v>7.0000000000000005E-8</v>
+      </c>
+      <c r="U21" s="24">
+        <f t="shared" si="10"/>
+        <v>7.2500000000000007E-8</v>
+      </c>
+      <c r="V21" s="24">
+        <f t="shared" si="10"/>
+        <v>7.500000000000001E-8</v>
+      </c>
+      <c r="W21" s="24">
+        <f t="shared" si="10"/>
+        <v>7.7500000000000012E-8</v>
+      </c>
+      <c r="X21" s="24">
+        <f t="shared" si="10"/>
+        <v>8.0000000000000002E-8</v>
+      </c>
+      <c r="Z21" s="27">
+        <f>SUM(L21:X21)</f>
+        <v>8.4500000000000006E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B22" s="9"/>
       <c r="D22" t="s">
         <v>38</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="24">
         <f>F18*F4*F13*F14</f>
-        <v>3.2500000000000001E-7</v>
+        <v>2.4999999999999999E-8</v>
       </c>
       <c r="F22">
         <f>F18</f>
@@ -1644,21 +1830,21 @@
       </c>
       <c r="G22">
         <f>E22*F6/F14*F15</f>
-        <v>1.6250000000000001E-10</v>
+        <v>1.2500000000000002E-11</v>
       </c>
       <c r="I22" s="11">
         <f>(E22+E23)/2</f>
-        <v>2.4375E-7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+        <v>1.8749999999999999E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B23" s="9"/>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23">
         <f>F19*F4*F13*F14</f>
-        <v>1.6250000000000001E-7</v>
+        <v>1.2499999999999999E-8</v>
       </c>
       <c r="F23">
         <f>F19</f>
@@ -1666,18 +1852,18 @@
       </c>
       <c r="G23" s="18">
         <f>E23*F6/F14*F15</f>
-        <v>8.1250000000000004E-11</v>
+        <v>6.250000000000001E-12</v>
       </c>
       <c r="I23" s="11">
         <f>(G22+G23)/2</f>
-        <v>1.2187500000000001E-10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+        <v>9.3750000000000016E-12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B24" s="9"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>52</v>
       </c>
@@ -1689,25 +1875,25 @@
       </c>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B26" s="9"/>
       <c r="D26" t="s">
         <v>38</v>
       </c>
       <c r="E26">
         <f>F22*F4*F14*F13</f>
-        <v>3.2499999999999996E-7</v>
+        <v>2.4999999999999999E-8</v>
       </c>
       <c r="G26">
         <f>E26*F6/F14*F15</f>
-        <v>1.6249999999999998E-10</v>
+        <v>1.2500000000000002E-11</v>
       </c>
       <c r="I26" s="11">
         <f>(E26+E27)/2</f>
-        <v>2.4375E-7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+        <v>1.8749999999999999E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21" t="s">
@@ -1715,17 +1901,17 @@
       </c>
       <c r="E27" s="21">
         <f>F23*F4*F14*F13</f>
-        <v>1.6249999999999998E-7</v>
+        <v>1.2499999999999999E-8</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21">
         <f>E27*F6/F14*F15</f>
-        <v>8.1249999999999991E-11</v>
+        <v>6.250000000000001E-12</v>
       </c>
       <c r="H27" s="21"/>
       <c r="I27" s="13">
         <f>(G26+G27)/2</f>
-        <v>1.2187499999999998E-10</v>
+        <v>9.3750000000000016E-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>